<commit_message>
added open , unzip, clearing when close
</commit_message>
<xml_diff>
--- a/aaaa.xlsx
+++ b/aaaa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +92,14 @@
   </si>
   <si>
     <t>아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdfz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zsd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,9 +455,9 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -475,7 +483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -501,7 +509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>100</v>
       </c>
@@ -541,9 +549,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -557,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -583,7 +591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>100</v>
       </c>
@@ -618,12 +626,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -634,13 +655,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -654,7 +675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -680,7 +701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
added multi cell read
</commit_message>
<xml_diff>
--- a/aaaa.xlsx
+++ b/aaaa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -636,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>